<commit_message>
feat: teste de sobreposição com sobreposição OK
</commit_message>
<xml_diff>
--- a/assets/dados_para_sobreposição_sem_sobreposição.xlsx
+++ b/assets/dados_para_sobreposição_sem_sobreposição.xlsx
@@ -14,9 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Elemento</t>
+  </si>
+  <si>
+    <t>h_x (m)</t>
+  </si>
+  <si>
+    <t>h_y (m)</t>
   </si>
   <si>
     <t>ap (m)</t>
@@ -147,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,6 +175,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -496,179 +505,191 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="8">
+        <v>18</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9">
         <v>0.5</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="9">
         <v>0.25</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="10">
         <v>10</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="9">
+        <v>19</v>
+      </c>
+      <c r="H2" s="10">
         <v>2</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="10">
         <v>2</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="10">
         <v>294</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="9">
         <v>58.8</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="9">
         <v>29.4</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="9">
         <v>511.6</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="9">
         <v>-32.4</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="9">
         <v>-0.4</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="9">
         <v>511.6</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="Q2" s="9">
         <v>-32.4</v>
       </c>
-      <c r="R2" s="8">
+      <c r="R2" s="9">
         <v>-0.4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="8">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9">
         <v>0.6</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>0.4</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="10">
         <v>25</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="9">
+        <v>19</v>
+      </c>
+      <c r="H3" s="10">
         <v>0</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="10">
         <v>0</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="10">
         <v>1040</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="10">
         <v>280</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="10">
         <v>190</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="10">
         <v>1040</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="10">
         <v>280</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="10">
         <v>190</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="10">
         <v>1040</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="Q3" s="10">
         <v>280</v>
       </c>
-      <c r="R3" s="9">
+      <c r="R3" s="10">
         <v>190</v>
       </c>
     </row>

</xml_diff>